<commit_message>
minor tweaks to XLS
</commit_message>
<xml_diff>
--- a/P2S-VPN-Calculator/P2S VPN calculator.xlsx
+++ b/P2S-VPN-Calculator/P2S VPN calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsoderholm\Git\public-azure\P2S-VPN-Calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2260FD-BF81-4E01-A2C2-3BCE9CBFF85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C20E4A-5A5E-423E-A332-0C0A33BEC5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26865" yWindow="3705" windowWidth="23370" windowHeight="15345" xr2:uid="{300EEF6A-A800-422E-B163-2E0CAA9786F4}"/>
+    <workbookView xWindow="465" yWindow="1320" windowWidth="25920" windowHeight="15480" xr2:uid="{300EEF6A-A800-422E-B163-2E0CAA9786F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,9 +116,6 @@
     <t>GB/month</t>
   </si>
   <si>
-    <t>Gateway pricing:</t>
-  </si>
-  <si>
     <t>VPN Gateway Pricing | Microsoft Azure</t>
   </si>
   <si>
@@ -126,16 +123,22 @@
   </si>
   <si>
     <t>Pricing Calculator | Microsoft Azure</t>
+  </si>
+  <si>
+    <t>soderholmd/public-azure (github.com)</t>
+  </si>
+  <si>
+    <t>This sheet comes with no guarantee of accuracy.</t>
   </si>
   <si>
     <t>Daniel Söderholm
 Microsoft UK
-Version 1.0 - 24/07/2023
+Version 1.1 - 20/12/2023
 MIT licence applies
 This sheet lives here: https://github.com/soderholmd/public-azure</t>
   </si>
   <si>
-    <t>soderholmd/public-azure (github.com)</t>
+    <t>Gateway pricing and size:</t>
   </si>
   <si>
     <r>
@@ -161,11 +164,8 @@
 1. Enter the number of connected users throughout the day on weekdays and weekends in the coloured boxes
 2. Check the average bandwidth per user (use existing VPN gateway/firewall logs if possible) in cell G4
 3. Check the Azure VPN pricing page to understand which gateway SKU is required for the number of users/bandwidth in cells L14/L15
-4. Enter the gateway SKU, billable P2S tunnels, and bandwidth into the Azure pricing calculator for a total cost</t>
+4. Enter the gateway SKU, billable P2S tunnels, and bandwidth into the Azure pricing calculator for a total cost (not including network egress fees)</t>
     </r>
-  </si>
-  <si>
-    <t>This sheet comes with no guarantee of accuracy.</t>
   </si>
 </sst>
 </file>
@@ -299,11 +299,10 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1911,26 +1910,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B024EBBD-47BE-4452-AFEB-0CF616A01735}">
   <dimension ref="B2:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
-    <col min="7" max="10" width="15.42578125" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="25.1796875" customWidth="1"/>
+    <col min="7" max="10" width="15.453125" customWidth="1"/>
+    <col min="11" max="11" width="22.81640625" customWidth="1"/>
+    <col min="13" max="13" width="10.7265625" customWidth="1"/>
+    <col min="14" max="14" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C2" s="22" t="s">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="C2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="22"/>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1941,14 +1940,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" s="4">
-        <v>700</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="C4" s="3">
+        <v>700</v>
+      </c>
+      <c r="D4" s="3">
         <v>700</v>
       </c>
       <c r="F4" t="s">
@@ -1961,25 +1960,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="4">
-        <v>700</v>
-      </c>
-      <c r="D5" s="4">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C5" s="3">
+        <v>700</v>
+      </c>
+      <c r="D5" s="3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="4">
-        <v>700</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="C6" s="3">
+        <v>700</v>
+      </c>
+      <c r="D6" s="3">
         <v>700</v>
       </c>
       <c r="G6" t="s">
@@ -1998,512 +1997,512 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>3</v>
       </c>
-      <c r="C7" s="4">
-        <v>700</v>
-      </c>
-      <c r="D7" s="4">
-        <v>700</v>
-      </c>
-      <c r="F7" s="17" t="s">
+      <c r="C7" s="3">
+        <v>700</v>
+      </c>
+      <c r="D7" s="3">
+        <v>700</v>
+      </c>
+      <c r="F7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="9">
-        <f>AVERAGE(C4:C9,C24:C27,D4:D12,D20:D27)</f>
-        <v>711.11111111111109</v>
-      </c>
-      <c r="H7" s="8">
+      <c r="G7" s="8">
+        <f>AVERAGE(C4:C9,C24:C27,D4:D12,D21:D27)</f>
+        <v>700</v>
+      </c>
+      <c r="H7" s="7">
         <v>82</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="8">
         <f>G7*H7</f>
-        <v>58311.111111111109</v>
-      </c>
-      <c r="J7" s="9">
+        <v>57400</v>
+      </c>
+      <c r="J7" s="8">
         <f>G7*G$4</f>
-        <v>355.55555555555554</v>
-      </c>
-      <c r="K7" s="9">
+        <v>350</v>
+      </c>
+      <c r="K7" s="8">
         <f>(J7*H7*3600)/1024/8</f>
-        <v>12812.5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+        <v>12612.3046875</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8" s="4">
-        <v>700</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="C8" s="3">
+        <v>700</v>
+      </c>
+      <c r="D8" s="3">
         <v>700</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="9">
-        <f>AVERAGE(C10:C12,C21:C23,D13:D19)</f>
-        <v>1461.5384615384614</v>
-      </c>
-      <c r="H8" s="8">
+      <c r="G8" s="8">
+        <f>AVERAGE(C10:C12,C21:C23,D13:D20)</f>
+        <v>1428.5714285714287</v>
+      </c>
+      <c r="H8" s="7">
         <v>46</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="8">
         <f t="shared" ref="I8:I9" si="0">G8*H8</f>
-        <v>67230.76923076922</v>
-      </c>
-      <c r="J8" s="9">
+        <v>65714.285714285725</v>
+      </c>
+      <c r="J8" s="8">
         <f t="shared" ref="J8:J9" si="1">G8*G$4</f>
-        <v>730.76923076923072</v>
-      </c>
-      <c r="K8" s="9">
+        <v>714.28571428571433</v>
+      </c>
+      <c r="K8" s="8">
         <f t="shared" ref="K8:K9" si="2">(J8*H8*3600)/1024/8</f>
-        <v>14772.38581730769</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+        <v>14439.174107142859</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>5</v>
       </c>
-      <c r="C9" s="4">
-        <v>700</v>
-      </c>
-      <c r="D9" s="4">
-        <v>700</v>
-      </c>
-      <c r="F9" s="18" t="s">
+      <c r="C9" s="3">
+        <v>700</v>
+      </c>
+      <c r="D9" s="3">
+        <v>700</v>
+      </c>
+      <c r="F9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="12">
         <f>AVERAGE(C13:C20)</f>
         <v>3500</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="13">
         <v>40</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="12">
         <f t="shared" si="0"/>
         <v>140000</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="12">
         <f t="shared" si="1"/>
         <v>1750</v>
       </c>
-      <c r="K9" s="13">
+      <c r="K9" s="12">
         <f t="shared" si="2"/>
         <v>30761.71875</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>6</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>1250</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>700</v>
       </c>
       <c r="F10" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="10">
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="9">
         <f>SUM(I7:I9)</f>
-        <v>265541.88034188031</v>
-      </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="9">
+        <v>263114.28571428574</v>
+      </c>
+      <c r="J10" s="6"/>
+      <c r="K10" s="8">
         <f>SUM(K7:K9)</f>
-        <v>58346.604567307688</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+        <v>57813.197544642855</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>7</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>2000</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>700</v>
       </c>
       <c r="F11" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="10">
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="9">
         <f>I10*4.33</f>
-        <v>1149796.3418803418</v>
-      </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="9">
+        <v>1139284.8571428573</v>
+      </c>
+      <c r="J11" s="7"/>
+      <c r="K11" s="8">
         <f>K10*4.333</f>
-        <v>252815.83759014422</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+        <v>250504.5849609375</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>8</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>2750</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>700</v>
       </c>
       <c r="F12" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="10">
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="9">
         <f>I11/730</f>
-        <v>1575.0634820278653</v>
-      </c>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+        <v>1560.6641878669277</v>
+      </c>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>9</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>3500</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>1000</v>
       </c>
-      <c r="K13" s="16" t="s">
+      <c r="K13" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>10</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>3500</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>1000</v>
       </c>
       <c r="K14" t="s">
         <v>18</v>
       </c>
-      <c r="L14" s="11">
+      <c r="L14" s="10">
         <f>MAX(G7:G9)</f>
         <v>3500</v>
       </c>
-      <c r="M14" s="19" t="s">
+      <c r="M14" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="N14" s="15" t="s">
+      <c r="N14" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>11</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>3500</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>1000</v>
       </c>
       <c r="K15" t="s">
         <v>19</v>
       </c>
-      <c r="L15" s="11">
+      <c r="L15" s="10">
         <f>MAX(J7:J9)</f>
         <v>1750</v>
       </c>
-      <c r="M15" s="19" t="s">
+      <c r="M15" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="N15" s="15" t="s">
+      <c r="N15" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>12</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>3500</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>1000</v>
       </c>
       <c r="K16" t="s">
         <v>17</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="11">
         <f>K11</f>
-        <v>252815.83759014422</v>
-      </c>
-      <c r="M16" s="20" t="s">
+        <v>250504.5849609375</v>
+      </c>
+      <c r="M16" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="N16" s="15" t="s">
+      <c r="N16" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>13</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>3500</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>1000</v>
       </c>
       <c r="K17" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="12">
+      <c r="L17" s="11">
         <f>I12-128</f>
-        <v>1447.0634820278653</v>
-      </c>
-      <c r="M17" s="20"/>
-      <c r="N17" s="15" t="s">
+        <v>1432.6641878669277</v>
+      </c>
+      <c r="M17" s="19"/>
+      <c r="N17" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>14</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>3500</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>1000</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>15</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>3500</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>16</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>3500</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <v>1000</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B21">
         <v>17</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="4">
         <v>2750</v>
       </c>
-      <c r="D21" s="4">
-        <v>700</v>
-      </c>
-      <c r="K21" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D21" s="3">
+        <v>700</v>
+      </c>
+      <c r="K21" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B22">
         <v>18</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <v>2000</v>
       </c>
-      <c r="D22" s="4">
-        <v>700</v>
-      </c>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="24"/>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D22" s="3">
+        <v>700</v>
+      </c>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>19</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>1250</v>
       </c>
-      <c r="D23" s="4">
-        <v>700</v>
-      </c>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="24"/>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D23" s="3">
+        <v>700</v>
+      </c>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B24">
         <v>20</v>
       </c>
-      <c r="C24" s="4">
-        <v>700</v>
-      </c>
-      <c r="D24" s="4">
+      <c r="C24" s="3">
+        <v>700</v>
+      </c>
+      <c r="D24" s="3">
         <v>700</v>
       </c>
       <c r="J24" s="2"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="24"/>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B25">
         <v>21</v>
       </c>
-      <c r="C25" s="4">
-        <v>700</v>
-      </c>
-      <c r="D25" s="4">
-        <v>700</v>
-      </c>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="24"/>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C25" s="3">
+        <v>700</v>
+      </c>
+      <c r="D25" s="3">
+        <v>700</v>
+      </c>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B26">
         <v>22</v>
       </c>
-      <c r="C26" s="4">
-        <v>700</v>
-      </c>
-      <c r="D26" s="4">
-        <v>700</v>
-      </c>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24"/>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C26" s="3">
+        <v>700</v>
+      </c>
+      <c r="D26" s="3">
+        <v>700</v>
+      </c>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B27">
         <v>23</v>
       </c>
-      <c r="C27" s="4">
-        <v>700</v>
-      </c>
-      <c r="D27" s="4">
-        <v>700</v>
-      </c>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="24"/>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="24"/>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="24"/>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
-    </row>
-    <row r="32" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="25" t="s">
+      <c r="C27" s="3">
+        <v>700</v>
+      </c>
+      <c r="D27" s="3">
+        <v>700</v>
+      </c>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="K31" s="23"/>
+      <c r="L31" s="23"/>
+      <c r="M31" s="23"/>
+      <c r="N31" s="23"/>
+    </row>
+    <row r="32" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="K34" t="s">
+        <v>32</v>
+      </c>
+      <c r="L34" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="K35" t="s">
+        <v>27</v>
+      </c>
+      <c r="L35" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B37" s="24"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B38" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
         <v>30</v>
-      </c>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="K32" s="24"/>
-      <c r="L32" s="24"/>
-      <c r="M32" s="24"/>
-      <c r="N32" s="24"/>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="K34" t="s">
-        <v>26</v>
-      </c>
-      <c r="L34" s="21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="K35" t="s">
-        <v>28</v>
-      </c>
-      <c r="L35" s="21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2518,9 +2517,6 @@
     <hyperlink ref="B38" r:id="rId3" display="https://github.com/soderholmd/public-azure" xr:uid="{91004617-9681-468E-8472-DA9DD044BCBE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="G9" formulaRange="1"/>
-  </ignoredErrors>
   <drawing r:id="rId4"/>
 </worksheet>
 </file>

</xml_diff>